<commit_message>
Ajustes para la UX/UI
</commit_message>
<xml_diff>
--- a/cluster_means_report.xlsx
+++ b/cluster_means_report.xlsx
@@ -550,67 +550,67 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2431.384615384615</v>
+        <v>141.3076923076923</v>
       </c>
       <c r="C2" t="n">
-        <v>584.9807692307693</v>
+        <v>22.69230769230769</v>
       </c>
       <c r="D2" t="n">
-        <v>1199.865384615385</v>
+        <v>42.42307692307692</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4882115384615385</v>
+        <v>0.5413076923076923</v>
       </c>
       <c r="F2" t="n">
-        <v>142.5192307692308</v>
+        <v>2.615384615384615</v>
       </c>
       <c r="G2" t="n">
-        <v>389.9615384615385</v>
+        <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>0.359826923076923</v>
+        <v>0.1985</v>
       </c>
       <c r="I2" t="n">
-        <v>307.3461538461539</v>
+        <v>9.307692307692308</v>
       </c>
       <c r="J2" t="n">
-        <v>378.2307692307692</v>
+        <v>13.73076923076923</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8166346153846153</v>
+        <v>0.6404615384615385</v>
       </c>
       <c r="L2" t="n">
-        <v>87.48076923076923</v>
+        <v>14.34615384615385</v>
       </c>
       <c r="M2" t="n">
-        <v>378.7884615384615</v>
+        <v>27.84615384615385</v>
       </c>
       <c r="N2" t="n">
-        <v>466.2692307692308</v>
+        <v>42.19230769230769</v>
       </c>
       <c r="O2" t="n">
-        <v>387.1923076923077</v>
+        <v>10.61538461538461</v>
       </c>
       <c r="P2" t="n">
-        <v>77.69230769230769</v>
+        <v>4.653846153846154</v>
       </c>
       <c r="Q2" t="n">
-        <v>53.82692307692308</v>
+        <v>5.307692307692307</v>
       </c>
       <c r="R2" t="n">
-        <v>179.2115384615385</v>
+        <v>7.692307692307693</v>
       </c>
       <c r="S2" t="n">
-        <v>159.1346153846154</v>
+        <v>16.38461538461538</v>
       </c>
       <c r="T2" t="n">
-        <v>1619.826923076923</v>
+        <v>57.30769230769231</v>
       </c>
       <c r="U2" t="n">
-        <v>71.76923076923077</v>
+        <v>5.461538461538462</v>
       </c>
       <c r="V2" t="n">
-        <v>70.40384615384616</v>
+        <v>4.038461538461538</v>
       </c>
     </row>
     <row r="3">
@@ -618,67 +618,67 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>384.7123287671233</v>
+        <v>122.9298245614035</v>
       </c>
       <c r="C3" t="n">
-        <v>51.65068493150685</v>
+        <v>17.40350877192983</v>
       </c>
       <c r="D3" t="n">
-        <v>114.472602739726</v>
+        <v>37.66666666666666</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4526506849315069</v>
+        <v>0.4620350877192982</v>
       </c>
       <c r="F3" t="n">
-        <v>14.47260273972603</v>
+        <v>7.087719298245614</v>
       </c>
       <c r="G3" t="n">
-        <v>44.45205479452055</v>
+        <v>19.05263157894737</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2732876712328767</v>
+        <v>0.3646491228070176</v>
       </c>
       <c r="I3" t="n">
-        <v>18.32191780821918</v>
+        <v>7.87719298245614</v>
       </c>
       <c r="J3" t="n">
-        <v>25.82876712328767</v>
+        <v>9.842105263157896</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7137397260273973</v>
+        <v>0.8077017543859649</v>
       </c>
       <c r="L3" t="n">
-        <v>22.01369863013699</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="M3" t="n">
-        <v>50.71917808219178</v>
+        <v>13.08771929824561</v>
       </c>
       <c r="N3" t="n">
-        <v>72.73287671232876</v>
+        <v>17.42105263157895</v>
       </c>
       <c r="O3" t="n">
-        <v>34.52739726027397</v>
+        <v>12.19298245614035</v>
       </c>
       <c r="P3" t="n">
-        <v>12.44520547945205</v>
+        <v>4.210526315789473</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.712328767123287</v>
+        <v>1.578947368421053</v>
       </c>
       <c r="R3" t="n">
-        <v>18.25342465753425</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="S3" t="n">
-        <v>35.06849315068493</v>
+        <v>10.89473684210526</v>
       </c>
       <c r="T3" t="n">
-        <v>136.0958904109589</v>
+        <v>49.7719298245614</v>
       </c>
       <c r="U3" t="n">
-        <v>28.82876712328767</v>
+        <v>5.035087719298246</v>
       </c>
       <c r="V3" t="n">
-        <v>3.856164383561644</v>
+        <v>2.035087719298246</v>
       </c>
     </row>
     <row r="4">
@@ -686,67 +686,67 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1104.801418439716</v>
+        <v>161.5416666666667</v>
       </c>
       <c r="C4" t="n">
-        <v>159.9290780141844</v>
+        <v>38.20833333333334</v>
       </c>
       <c r="D4" t="n">
-        <v>355.7730496453901</v>
+        <v>73.91666666666667</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4514609929078014</v>
+        <v>0.5199583333333333</v>
       </c>
       <c r="F4" t="n">
-        <v>61.56737588652482</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
-        <v>168.3475177304965</v>
+        <v>21</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3705106382978723</v>
+        <v>0.3650416666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>56.11347517730496</v>
+        <v>24.5</v>
       </c>
       <c r="J4" t="n">
-        <v>72.36879432624113</v>
+        <v>32.79166666666666</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7720567375886525</v>
+        <v>0.7587083333333333</v>
       </c>
       <c r="L4" t="n">
-        <v>41.29078014184397</v>
+        <v>9.125</v>
       </c>
       <c r="M4" t="n">
-        <v>129.8723404255319</v>
+        <v>36.41666666666666</v>
       </c>
       <c r="N4" t="n">
-        <v>171.1631205673759</v>
+        <v>45.54166666666666</v>
       </c>
       <c r="O4" t="n">
-        <v>113.4255319148936</v>
+        <v>21.79166666666667</v>
       </c>
       <c r="P4" t="n">
-        <v>35.86524822695036</v>
+        <v>5.708333333333333</v>
       </c>
       <c r="Q4" t="n">
-        <v>18.75177304964539</v>
+        <v>5.083333333333333</v>
       </c>
       <c r="R4" t="n">
-        <v>50.53191489361702</v>
+        <v>13.75</v>
       </c>
       <c r="S4" t="n">
-        <v>86.93617021276596</v>
+        <v>14.41666666666667</v>
       </c>
       <c r="T4" t="n">
-        <v>437.5390070921986</v>
+        <v>108.9166666666667</v>
       </c>
       <c r="U4" t="n">
-        <v>54.31205673758866</v>
+        <v>4.916666666666667</v>
       </c>
       <c r="V4" t="n">
-        <v>16.15602836879433</v>
+        <v>4.916666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -754,67 +754,67 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1537.028571428571</v>
+        <v>169.2448979591837</v>
       </c>
       <c r="C5" t="n">
-        <v>268.5142857142857</v>
+        <v>28.79591836734694</v>
       </c>
       <c r="D5" t="n">
-        <v>447.5714285714286</v>
+        <v>66.18367346938776</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6116857142857143</v>
+        <v>0.4376530612244898</v>
       </c>
       <c r="F5" t="n">
-        <v>9.285714285714286</v>
+        <v>11.63265306122449</v>
       </c>
       <c r="G5" t="n">
-        <v>34.48571428571429</v>
+        <v>33</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1327714285714286</v>
+        <v>0.3561224489795918</v>
       </c>
       <c r="I5" t="n">
-        <v>103.9142857142857</v>
+        <v>12</v>
       </c>
       <c r="J5" t="n">
-        <v>153.3142857142857</v>
+        <v>14.93877551020408</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6727428571428571</v>
+        <v>0.7896734693877552</v>
       </c>
       <c r="L5" t="n">
-        <v>167.6571428571428</v>
+        <v>5.163265306122449</v>
       </c>
       <c r="M5" t="n">
-        <v>334.8857142857143</v>
+        <v>18.40816326530612</v>
       </c>
       <c r="N5" t="n">
-        <v>502.5428571428571</v>
+        <v>23.57142857142857</v>
       </c>
       <c r="O5" t="n">
-        <v>109.3714285714286</v>
+        <v>18.3265306122449</v>
       </c>
       <c r="P5" t="n">
-        <v>43.57142857142857</v>
+        <v>6.122448979591836</v>
       </c>
       <c r="Q5" t="n">
-        <v>71.71428571428571</v>
+        <v>2.346938775510204</v>
       </c>
       <c r="R5" t="n">
-        <v>77.97142857142858</v>
+        <v>8.836734693877551</v>
       </c>
       <c r="S5" t="n">
-        <v>157.5714285714286</v>
+        <v>13.20408163265306</v>
       </c>
       <c r="T5" t="n">
-        <v>650.2285714285714</v>
+        <v>81.22448979591837</v>
       </c>
       <c r="U5" t="n">
-        <v>65.57142857142857</v>
+        <v>5.489795918367347</v>
       </c>
       <c r="V5" t="n">
-        <v>39.14285714285715</v>
+        <v>4.346938775510204</v>
       </c>
     </row>
     <row r="6">
@@ -822,67 +822,67 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1991.416666666667</v>
+        <v>186.9583333333333</v>
       </c>
       <c r="C6" t="n">
-        <v>344.8333333333333</v>
+        <v>47.33333333333334</v>
       </c>
       <c r="D6" t="n">
-        <v>747.5648148148148</v>
+        <v>96.79166666666667</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4625555555555556</v>
+        <v>0.48775</v>
       </c>
       <c r="F6" t="n">
-        <v>131.1296296296296</v>
+        <v>14.25</v>
       </c>
       <c r="G6" t="n">
-        <v>346.7685185185185</v>
+        <v>37.95833333333334</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3745462962962963</v>
+        <v>0.3768333333333334</v>
       </c>
       <c r="I6" t="n">
-        <v>121.1574074074074</v>
+        <v>33.125</v>
       </c>
       <c r="J6" t="n">
-        <v>149.5462962962963</v>
+        <v>38.5</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8055648148148149</v>
+        <v>0.8590416666666667</v>
       </c>
       <c r="L6" t="n">
-        <v>63.6574074074074</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="M6" t="n">
-        <v>235.9907407407407</v>
+        <v>21.79166666666667</v>
       </c>
       <c r="N6" t="n">
-        <v>299.6481481481482</v>
+        <v>26.125</v>
       </c>
       <c r="O6" t="n">
-        <v>213.3611111111111</v>
+        <v>30.91666666666667</v>
       </c>
       <c r="P6" t="n">
-        <v>58.37037037037037</v>
+        <v>5.791666666666667</v>
       </c>
       <c r="Q6" t="n">
-        <v>33.55555555555556</v>
+        <v>2.458333333333333</v>
       </c>
       <c r="R6" t="n">
-        <v>99.86111111111111</v>
+        <v>15.58333333333333</v>
       </c>
       <c r="S6" t="n">
-        <v>144.6666666666667</v>
+        <v>13.41666666666667</v>
       </c>
       <c r="T6" t="n">
-        <v>941.9537037037037</v>
+        <v>142.0416666666667</v>
       </c>
       <c r="U6" t="n">
-        <v>69.73148148148148</v>
+        <v>5.5</v>
       </c>
       <c r="V6" t="n">
-        <v>47.58333333333334</v>
+        <v>5.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>